<commit_message>
Implemented fixes and suggestions to code. Added functions and worked on calculations in main. Made edits to excel files and added project specs file.
</commit_message>
<xml_diff>
--- a/RunLog.xlsx
+++ b/RunLog.xlsx
@@ -1,43 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adoyn\Documents\School\Grad School Courses\Summer 2024\HCI 584X\Project\Running_Log_App\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC895065-A24C-4033-95B9-3DED042AA966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="570" windowWidth="24810" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -52,43 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -376,31 +424,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Run Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Hours</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Minutes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Seconds</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Miles</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pace</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45292</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>61.01666666666667</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45293</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>31.01666666666667</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45294</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
+        <v>15.17083333333333</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45295</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>61.01666666666667</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45296</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>18.305</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Incorporated some suggestions to main.py. Worked on majority of user functionality. Updated data in excel spreadsheet.
</commit_message>
<xml_diff>
--- a/RunLog.xlsx
+++ b/RunLog.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,19 +484,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>16.1</v>
       </c>
       <c r="G2" t="n">
-        <v>61.01666666666667</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -509,19 +509,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>13.2</v>
       </c>
       <c r="G3" t="n">
-        <v>31.01666666666667</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -534,19 +534,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>17.5</v>
       </c>
       <c r="G4" t="n">
-        <v>15.17083333333333</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -559,19 +559,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F5" t="n">
-        <v>4</v>
+        <v>21.3</v>
       </c>
       <c r="G5" t="n">
-        <v>61.01666666666667</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -584,19 +584,94 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>15.6</v>
       </c>
       <c r="G6" t="n">
-        <v>18.305</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45297</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>42</v>
+      </c>
+      <c r="F7" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="G7" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45298</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45299</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>25.9</v>
+      </c>
+      <c r="G9" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed editing section. Added load, save as, and save. Cleaned up comments in code. Added dummy data to excel file.
</commit_message>
<xml_diff>
--- a/RunLog.xlsx
+++ b/RunLog.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -674,6 +674,731 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45300</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="G10" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45301</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7</v>
+      </c>
+      <c r="E11" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G11" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45302</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>32</v>
+      </c>
+      <c r="E12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F12" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45303</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>32</v>
+      </c>
+      <c r="E13" t="n">
+        <v>20</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45304</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>6</v>
+      </c>
+      <c r="D14" t="n">
+        <v>32</v>
+      </c>
+      <c r="E14" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45305</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>32</v>
+      </c>
+      <c r="E15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F15" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45306</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>23</v>
+      </c>
+      <c r="E16" t="n">
+        <v>20</v>
+      </c>
+      <c r="F16" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45307</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>23</v>
+      </c>
+      <c r="E17" t="n">
+        <v>20</v>
+      </c>
+      <c r="F17" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="G17" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45308</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>23</v>
+      </c>
+      <c r="E18" t="n">
+        <v>20</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="G18" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45309</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" t="n">
+        <v>23</v>
+      </c>
+      <c r="E19" t="n">
+        <v>20</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="G19" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45310</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>23</v>
+      </c>
+      <c r="E20" t="n">
+        <v>20</v>
+      </c>
+      <c r="F20" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45311</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>23</v>
+      </c>
+      <c r="E21" t="n">
+        <v>20</v>
+      </c>
+      <c r="F21" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45312</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>32</v>
+      </c>
+      <c r="E22" t="n">
+        <v>20</v>
+      </c>
+      <c r="F22" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="G22" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45313</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="n">
+        <v>32</v>
+      </c>
+      <c r="E23" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G23" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45314</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="n">
+        <v>36</v>
+      </c>
+      <c r="E24" t="n">
+        <v>20</v>
+      </c>
+      <c r="F24" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="G24" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" t="n">
+        <v>36</v>
+      </c>
+      <c r="E25" t="n">
+        <v>20</v>
+      </c>
+      <c r="F25" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="G25" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45316</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>27</v>
+      </c>
+      <c r="E26" t="n">
+        <v>20</v>
+      </c>
+      <c r="F26" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="G26" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45317</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>27</v>
+      </c>
+      <c r="E27" t="n">
+        <v>20</v>
+      </c>
+      <c r="F27" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="G27" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45318</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>6</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="G28" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45319</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>6</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="G29" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45320</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="G30" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45321</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="G31" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45322</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45323</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="G33" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45324</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="G34" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45325</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="n">
+        <v>22</v>
+      </c>
+      <c r="E35" t="n">
+        <v>28</v>
+      </c>
+      <c r="F35" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="G35" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45326</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>22</v>
+      </c>
+      <c r="E36" t="n">
+        <v>28</v>
+      </c>
+      <c r="F36" t="n">
+        <v>10</v>
+      </c>
+      <c r="G36" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45331</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>road</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" t="n">
+        <v>17</v>
+      </c>
+      <c r="E37" t="n">
+        <v>19</v>
+      </c>
+      <c r="F37" t="n">
+        <v>10</v>
+      </c>
+      <c r="G37" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45332</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>trail</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="G38" t="n">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed spelling mistakes in comments. Update dummy data in excel.
</commit_message>
<xml_diff>
--- a/RunLog.xlsx
+++ b/RunLog.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1375,7 +1378,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="3" t="n">
         <v>45332</v>
       </c>
       <c r="B38" t="inlineStr">

</xml_diff>